<commit_message>
Update to task statistics
</commit_message>
<xml_diff>
--- a/Info/Tasks.xlsx
+++ b/Info/Tasks.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="202300"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vult-my.sharepoint.com/personal/tadas_riksas_mif_stud_vu_lt/Documents/Documents/Studijos/3 semestras/Software engineering/Lab/speed/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://vult-my.sharepoint.com/personal/tadas_riksas_mif_stud_vu_lt/Documents/Documents/Studijos/3 semestras/Software engineering/Lab/speed/Info/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="12" documentId="8_{2B03AB53-9C09-4A4E-8DFC-8C147B64B2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A1DF3FA8-91DE-4CB3-B5D8-F2954D9CDB8C}"/>
+  <xr:revisionPtr revIDLastSave="28" documentId="8_{2B03AB53-9C09-4A4E-8DFC-8C147B64B2F8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{BE5B16FE-308B-4A7B-A8DA-2B0D808F6A6B}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-1935" windowWidth="29040" windowHeight="18240" xr2:uid="{AF9452B6-C75A-4AC3-8E83-7D91FCD7B517}"/>
+    <workbookView xWindow="-21390" yWindow="-105" windowWidth="21600" windowHeight="11385" xr2:uid="{AF9452B6-C75A-4AC3-8E83-7D91FCD7B517}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="12">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="18">
   <si>
     <t>Task id</t>
   </si>
@@ -65,13 +65,31 @@
     <t xml:space="preserve">Info </t>
   </si>
   <si>
-    <t>Additional info on commits and task management</t>
-  </si>
-  <si>
     <t>-</t>
   </si>
   <si>
     <t>Name</t>
+  </si>
+  <si>
+    <t>Status</t>
+  </si>
+  <si>
+    <t>Done</t>
+  </si>
+  <si>
+    <t>Not done</t>
+  </si>
+  <si>
+    <t>Additional info on commits and task management, UML diagrams, logo</t>
+  </si>
+  <si>
+    <t>People</t>
+  </si>
+  <si>
+    <t>Time taken</t>
+  </si>
+  <si>
+    <t>Not necessary</t>
   </si>
 </sst>
 </file>
@@ -95,7 +113,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -108,8 +126,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="5" tint="0.59999389629810485"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -132,19 +156,32 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="5">
+  <cellXfs count="7">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
-      <alignment wrapText="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="1">
@@ -161,6 +198,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -480,10 +521,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2D543ED2-952D-4662-8620-4739A01EFD29}">
-  <dimension ref="A1:G40"/>
+  <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H24" sqref="H24"/>
+      <selection activeCell="G7" sqref="G7:H7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -494,44 +535,60 @@
     <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A1" s="3" t="s">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A1" s="4" t="s">
         <v>4</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
+      <c r="B1" s="4"/>
+      <c r="C1" s="4"/>
+      <c r="D1" s="4"/>
+      <c r="E1" s="4"/>
       <c r="G1" s="2" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="2" spans="1:7" x14ac:dyDescent="0.25">
-      <c r="A2" s="3"/>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
+      <c r="I1" s="5" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A2" s="4"/>
+      <c r="B2" s="4"/>
+      <c r="C2" s="4"/>
+      <c r="D2" s="4"/>
+      <c r="E2" s="4"/>
       <c r="G2" s="1" t="s">
         <v>6</v>
       </c>
-    </row>
-    <row r="3" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I2" s="1" t="s">
+        <v>12</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
-    </row>
-    <row r="4" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I3" s="1" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
-    </row>
-    <row r="8" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="I4" s="1"/>
+    </row>
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="G7" s="6" t="s">
+        <v>17</v>
+      </c>
+      <c r="H7" s="6"/>
+    </row>
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
       <c r="B8" s="2" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C8" s="2" t="s">
         <v>1</v>
@@ -542,245 +599,354 @@
       <c r="E8" s="2" t="s">
         <v>3</v>
       </c>
-    </row>
-    <row r="9" spans="1:7" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="F8" s="5" t="s">
+        <v>11</v>
+      </c>
+      <c r="G8" s="2" t="s">
+        <v>15</v>
+      </c>
+      <c r="H8" s="2" t="s">
+        <v>16</v>
+      </c>
+    </row>
+    <row r="9" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>1</v>
       </c>
       <c r="B9" s="1" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C9" s="1" t="str">
         <f>G4</f>
         <v xml:space="preserve">Info </v>
       </c>
-      <c r="D9" s="4" t="s">
+      <c r="D9" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="E9" s="1" t="s">
         <v>9</v>
       </c>
-      <c r="E9" s="1" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="10" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F9" s="1" t="str">
+        <f>I2</f>
+        <v>Done</v>
+      </c>
+      <c r="G9" s="1"/>
+      <c r="H9" s="1"/>
+    </row>
+    <row r="10" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A10" s="1"/>
       <c r="B10" s="1"/>
       <c r="C10" s="1"/>
       <c r="D10" s="1"/>
       <c r="E10" s="1"/>
-    </row>
-    <row r="11" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F10" s="1"/>
+      <c r="G10" s="1"/>
+      <c r="H10" s="1"/>
+    </row>
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1"/>
       <c r="B11" s="1"/>
       <c r="C11" s="1"/>
       <c r="D11" s="1"/>
       <c r="E11" s="1"/>
-    </row>
-    <row r="12" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F11" s="1"/>
+      <c r="G11" s="1"/>
+      <c r="H11" s="1"/>
+    </row>
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1"/>
       <c r="B12" s="1"/>
       <c r="C12" s="1"/>
       <c r="D12" s="1"/>
       <c r="E12" s="1"/>
-    </row>
-    <row r="13" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F12" s="1"/>
+      <c r="G12" s="1"/>
+      <c r="H12" s="1"/>
+    </row>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1"/>
       <c r="B13" s="1"/>
       <c r="C13" s="1"/>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
-    </row>
-    <row r="14" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F13" s="1"/>
+      <c r="G13" s="1"/>
+      <c r="H13" s="1"/>
+    </row>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
       <c r="D14" s="1"/>
       <c r="E14" s="1"/>
-    </row>
-    <row r="15" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F14" s="1"/>
+      <c r="G14" s="1"/>
+      <c r="H14" s="1"/>
+    </row>
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
       <c r="D15" s="1"/>
       <c r="E15" s="1"/>
-    </row>
-    <row r="16" spans="1:7" x14ac:dyDescent="0.25">
+      <c r="F15" s="1"/>
+      <c r="G15" s="1"/>
+      <c r="H15" s="1"/>
+    </row>
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
       <c r="D16" s="1"/>
       <c r="E16" s="1"/>
-    </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F16" s="1"/>
+      <c r="G16" s="1"/>
+      <c r="H16" s="1"/>
+    </row>
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
       <c r="D17" s="1"/>
       <c r="E17" s="1"/>
-    </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F17" s="1"/>
+      <c r="G17" s="1"/>
+      <c r="H17" s="1"/>
+    </row>
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
       <c r="D18" s="1"/>
       <c r="E18" s="1"/>
-    </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F18" s="1"/>
+      <c r="G18" s="1"/>
+      <c r="H18" s="1"/>
+    </row>
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
       <c r="D19" s="1"/>
       <c r="E19" s="1"/>
-    </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F19" s="1"/>
+      <c r="G19" s="1"/>
+      <c r="H19" s="1"/>
+    </row>
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
       <c r="D20" s="1"/>
       <c r="E20" s="1"/>
-    </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F20" s="1"/>
+      <c r="G20" s="1"/>
+      <c r="H20" s="1"/>
+    </row>
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
       <c r="D21" s="1"/>
       <c r="E21" s="1"/>
-    </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F21" s="1"/>
+      <c r="G21" s="1"/>
+      <c r="H21" s="1"/>
+    </row>
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
       <c r="D22" s="1"/>
       <c r="E22" s="1"/>
-    </row>
-    <row r="23" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F22" s="1"/>
+      <c r="G22" s="1"/>
+      <c r="H22" s="1"/>
+    </row>
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
       <c r="D23" s="1"/>
       <c r="E23" s="1"/>
-    </row>
-    <row r="24" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F23" s="1"/>
+      <c r="G23" s="1"/>
+      <c r="H23" s="1"/>
+    </row>
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
       <c r="D24" s="1"/>
       <c r="E24" s="1"/>
-    </row>
-    <row r="25" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F24" s="1"/>
+      <c r="G24" s="1"/>
+      <c r="H24" s="1"/>
+    </row>
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
       <c r="D25" s="1"/>
       <c r="E25" s="1"/>
-    </row>
-    <row r="26" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F25" s="1"/>
+      <c r="G25" s="1"/>
+      <c r="H25" s="1"/>
+    </row>
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
       <c r="D26" s="1"/>
       <c r="E26" s="1"/>
-    </row>
-    <row r="27" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F26" s="1"/>
+      <c r="G26" s="1"/>
+      <c r="H26" s="1"/>
+    </row>
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
       <c r="D27" s="1"/>
       <c r="E27" s="1"/>
-    </row>
-    <row r="28" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F27" s="1"/>
+      <c r="G27" s="1"/>
+      <c r="H27" s="1"/>
+    </row>
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
       <c r="D28" s="1"/>
       <c r="E28" s="1"/>
-    </row>
-    <row r="29" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F28" s="1"/>
+      <c r="G28" s="1"/>
+      <c r="H28" s="1"/>
+    </row>
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
       <c r="D29" s="1"/>
       <c r="E29" s="1"/>
-    </row>
-    <row r="30" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F29" s="1"/>
+      <c r="G29" s="1"/>
+      <c r="H29" s="1"/>
+    </row>
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
       <c r="D30" s="1"/>
       <c r="E30" s="1"/>
-    </row>
-    <row r="31" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F30" s="1"/>
+      <c r="G30" s="1"/>
+      <c r="H30" s="1"/>
+    </row>
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
       <c r="D31" s="1"/>
       <c r="E31" s="1"/>
-    </row>
-    <row r="32" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F31" s="1"/>
+      <c r="G31" s="1"/>
+      <c r="H31" s="1"/>
+    </row>
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
       <c r="D32" s="1"/>
       <c r="E32" s="1"/>
-    </row>
-    <row r="33" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F32" s="1"/>
+      <c r="G32" s="1"/>
+      <c r="H32" s="1"/>
+    </row>
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
       <c r="D33" s="1"/>
       <c r="E33" s="1"/>
-    </row>
-    <row r="34" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F33" s="1"/>
+      <c r="G33" s="1"/>
+      <c r="H33" s="1"/>
+    </row>
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
       <c r="D34" s="1"/>
       <c r="E34" s="1"/>
-    </row>
-    <row r="35" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F34" s="1"/>
+      <c r="G34" s="1"/>
+      <c r="H34" s="1"/>
+    </row>
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
       <c r="D35" s="1"/>
       <c r="E35" s="1"/>
-    </row>
-    <row r="36" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F35" s="1"/>
+      <c r="G35" s="1"/>
+      <c r="H35" s="1"/>
+    </row>
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
       <c r="D36" s="1"/>
       <c r="E36" s="1"/>
-    </row>
-    <row r="37" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F36" s="1"/>
+      <c r="G36" s="1"/>
+      <c r="H36" s="1"/>
+    </row>
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
       <c r="D37" s="1"/>
       <c r="E37" s="1"/>
-    </row>
-    <row r="38" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F37" s="1"/>
+      <c r="G37" s="1"/>
+      <c r="H37" s="1"/>
+    </row>
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
       <c r="D38" s="1"/>
       <c r="E38" s="1"/>
-    </row>
-    <row r="39" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F38" s="1"/>
+      <c r="G38" s="1"/>
+      <c r="H38" s="1"/>
+    </row>
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
       <c r="D39" s="1"/>
       <c r="E39" s="1"/>
-    </row>
-    <row r="40" spans="1:5" x14ac:dyDescent="0.25">
+      <c r="F39" s="1"/>
+      <c r="G39" s="1"/>
+      <c r="H39" s="1"/>
+    </row>
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>
       <c r="D40" s="1"/>
       <c r="E40" s="1"/>
+      <c r="F40" s="1"/>
+      <c r="G40" s="1"/>
+      <c r="H40" s="1"/>
     </row>
   </sheetData>
-  <mergeCells count="1">
+  <mergeCells count="2">
     <mergeCell ref="A1:E2"/>
+    <mergeCell ref="G7:H7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Added task txt file
</commit_message>
<xml_diff>
--- a/Info/Tasks.xlsx
+++ b/Info/Tasks.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\GitHub\speed\Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topto\OneDrive - Vilnius University\Documents\Studijos\3 semestras\Software engineering\speed\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98412787-CAD1-45A9-AB76-EAA224A5DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21390" yWindow="-105" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="3810" yWindow="2490" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="23">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Task id</t>
   </si>
@@ -104,13 +105,16 @@
   </si>
   <si>
     <t>Add new tasks</t>
+  </si>
+  <si>
+    <t>Create UI for the program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -199,7 +203,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -212,10 +216,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -534,22 +534,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="E11" sqref="E11"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.25" customWidth="1"/>
-    <col min="3" max="4" width="22.875" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -564,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -577,7 +577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
@@ -585,19 +585,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -623,7 +623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45.75" customHeight="1">
+    <row r="9" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -645,7 +645,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="42.75">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -665,7 +665,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -683,7 +683,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -701,17 +701,23 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9">
-      <c r="A13" s="1"/>
-      <c r="B13" s="1"/>
-      <c r="C13" s="1"/>
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A13" s="1">
+        <v>4</v>
+      </c>
+      <c r="B13" s="1" t="s">
+        <v>9</v>
+      </c>
+      <c r="C13" s="1" t="s">
+        <v>23</v>
+      </c>
       <c r="D13" s="1"/>
       <c r="E13" s="1"/>
       <c r="F13" s="1"/>
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:9">
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A14" s="1"/>
       <c r="B14" s="1"/>
       <c r="C14" s="1"/>
@@ -721,7 +727,7 @@
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -731,7 +737,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -741,7 +747,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -751,7 +757,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -761,7 +767,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -771,7 +777,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -781,7 +787,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -791,7 +797,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -801,7 +807,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -811,7 +817,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -821,7 +827,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -831,7 +837,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -841,7 +847,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -851,7 +857,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -861,7 +867,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -871,7 +877,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -881,7 +887,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -891,7 +897,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -901,7 +907,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -911,7 +917,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -921,7 +927,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -931,7 +937,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -941,7 +947,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -951,7 +957,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -961,7 +967,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -971,7 +977,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>

<commit_message>
Switch from blazor (#14)
* Added task txt file

* Changed folder structure, files...
</commit_message>
<xml_diff>
--- a/Info/Tasks.xlsx
+++ b/Info/Tasks.xlsx
@@ -1,20 +1,21 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="7" rupBuild="14420"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="27928"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\adria\Documents\GitHub\speed\Info\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\topto\OneDrive - Vilnius University\Documents\Studijos\3 semestras\Software engineering\speed\Info\"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{98412787-CAD1-45A9-AB76-EAA224A5DCAE}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-21390" yWindow="-105" windowWidth="21600" windowHeight="11385"/>
+    <workbookView xWindow="3810" yWindow="2490" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Lapas1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
@@ -35,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="26">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="31" uniqueCount="24">
   <si>
     <t>Task id</t>
   </si>
@@ -106,20 +107,14 @@
     <t>Add new tasks</t>
   </si>
   <si>
-    <t>Uzimtas?</t>
-  </si>
-  <si>
-    <t>Concepts</t>
-  </si>
-  <si>
-    <t>Visualising ideas</t>
+    <t>Create UI for the program</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <fonts count="2">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+  <fonts count="2" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -208,7 +203,7 @@
     </xf>
   </cellXfs>
   <cellStyles count="1">
-    <cellStyle name="Normal" xfId="0" builtinId="0"/>
+    <cellStyle name="Įprastas" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium2" defaultPivotStyle="PivotStyleLight16"/>
@@ -221,10 +216,6 @@
     </ext>
   </extLst>
 </styleSheet>
-</file>
-
-<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
-<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -543,22 +534,22 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:I40"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D14" sqref="D14"/>
+      <selection activeCell="E9" sqref="E9"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.25"/>
+  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="1" max="2" width="14.25" customWidth="1"/>
-    <col min="3" max="4" width="22.875" customWidth="1"/>
+    <col min="1" max="2" width="14.28515625" customWidth="1"/>
+    <col min="3" max="4" width="22.85546875" customWidth="1"/>
     <col min="5" max="5" width="61" customWidth="1"/>
-    <col min="7" max="7" width="15.875" customWidth="1"/>
+    <col min="7" max="7" width="15.85546875" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:9">
+    <row r="1" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A1" s="5" t="s">
         <v>4</v>
       </c>
@@ -573,7 +564,7 @@
         <v>11</v>
       </c>
     </row>
-    <row r="2" spans="1:9">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A2" s="5"/>
       <c r="B2" s="5"/>
       <c r="C2" s="5"/>
@@ -586,7 +577,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:9">
+    <row r="3" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G3" s="1" t="s">
         <v>7</v>
       </c>
@@ -594,19 +585,19 @@
         <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:9">
+    <row r="4" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G4" s="1" t="s">
         <v>8</v>
       </c>
       <c r="I4" s="1"/>
     </row>
-    <row r="7" spans="1:9">
+    <row r="7" spans="1:9" x14ac:dyDescent="0.25">
       <c r="G7" s="6" t="s">
         <v>17</v>
       </c>
       <c r="H7" s="6"/>
     </row>
-    <row r="8" spans="1:9">
+    <row r="8" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
         <v>0</v>
       </c>
@@ -632,7 +623,7 @@
         <v>16</v>
       </c>
     </row>
-    <row r="9" spans="1:9" ht="45.75" customHeight="1">
+    <row r="9" spans="1:9" ht="45.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A9" s="1">
         <v>0</v>
       </c>
@@ -654,7 +645,7 @@
       <c r="G9" s="1"/>
       <c r="H9" s="1"/>
     </row>
-    <row r="10" spans="1:9" ht="42.75">
+    <row r="10" spans="1:9" ht="60" x14ac:dyDescent="0.25">
       <c r="A10" s="1">
         <v>1</v>
       </c>
@@ -674,7 +665,7 @@
       <c r="G10" s="1"/>
       <c r="H10" s="1"/>
     </row>
-    <row r="11" spans="1:9">
+    <row r="11" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A11" s="1">
         <v>2</v>
       </c>
@@ -692,7 +683,7 @@
       <c r="G11" s="1"/>
       <c r="H11" s="1"/>
     </row>
-    <row r="12" spans="1:9">
+    <row r="12" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A12" s="1">
         <v>3</v>
       </c>
@@ -710,7 +701,7 @@
       <c r="G12" s="1"/>
       <c r="H12" s="1"/>
     </row>
-    <row r="13" spans="1:9">
+    <row r="13" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A13" s="1">
         <v>4</v>
       </c>
@@ -726,25 +717,17 @@
       <c r="G13" s="1"/>
       <c r="H13" s="1"/>
     </row>
-    <row r="14" spans="1:9">
-      <c r="A14" s="1">
-        <v>5</v>
-      </c>
-      <c r="B14" s="1" t="s">
-        <v>9</v>
-      </c>
-      <c r="C14" s="1" t="s">
-        <v>24</v>
-      </c>
-      <c r="D14" s="1" t="s">
-        <v>25</v>
-      </c>
+    <row r="14" spans="1:9" x14ac:dyDescent="0.25">
+      <c r="A14" s="1"/>
+      <c r="B14" s="1"/>
+      <c r="C14" s="1"/>
+      <c r="D14" s="1"/>
       <c r="E14" s="1"/>
       <c r="F14" s="1"/>
       <c r="G14" s="1"/>
       <c r="H14" s="1"/>
     </row>
-    <row r="15" spans="1:9">
+    <row r="15" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A15" s="1"/>
       <c r="B15" s="1"/>
       <c r="C15" s="1"/>
@@ -754,7 +737,7 @@
       <c r="G15" s="1"/>
       <c r="H15" s="1"/>
     </row>
-    <row r="16" spans="1:9">
+    <row r="16" spans="1:9" x14ac:dyDescent="0.25">
       <c r="A16" s="1"/>
       <c r="B16" s="1"/>
       <c r="C16" s="1"/>
@@ -764,7 +747,7 @@
       <c r="G16" s="1"/>
       <c r="H16" s="1"/>
     </row>
-    <row r="17" spans="1:8">
+    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A17" s="1"/>
       <c r="B17" s="1"/>
       <c r="C17" s="1"/>
@@ -774,7 +757,7 @@
       <c r="G17" s="1"/>
       <c r="H17" s="1"/>
     </row>
-    <row r="18" spans="1:8">
+    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A18" s="1"/>
       <c r="B18" s="1"/>
       <c r="C18" s="1"/>
@@ -784,7 +767,7 @@
       <c r="G18" s="1"/>
       <c r="H18" s="1"/>
     </row>
-    <row r="19" spans="1:8">
+    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A19" s="1"/>
       <c r="B19" s="1"/>
       <c r="C19" s="1"/>
@@ -794,7 +777,7 @@
       <c r="G19" s="1"/>
       <c r="H19" s="1"/>
     </row>
-    <row r="20" spans="1:8">
+    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A20" s="1"/>
       <c r="B20" s="1"/>
       <c r="C20" s="1"/>
@@ -804,7 +787,7 @@
       <c r="G20" s="1"/>
       <c r="H20" s="1"/>
     </row>
-    <row r="21" spans="1:8">
+    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A21" s="1"/>
       <c r="B21" s="1"/>
       <c r="C21" s="1"/>
@@ -814,7 +797,7 @@
       <c r="G21" s="1"/>
       <c r="H21" s="1"/>
     </row>
-    <row r="22" spans="1:8">
+    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A22" s="1"/>
       <c r="B22" s="1"/>
       <c r="C22" s="1"/>
@@ -824,7 +807,7 @@
       <c r="G22" s="1"/>
       <c r="H22" s="1"/>
     </row>
-    <row r="23" spans="1:8">
+    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A23" s="1"/>
       <c r="B23" s="1"/>
       <c r="C23" s="1"/>
@@ -834,7 +817,7 @@
       <c r="G23" s="1"/>
       <c r="H23" s="1"/>
     </row>
-    <row r="24" spans="1:8">
+    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A24" s="1"/>
       <c r="B24" s="1"/>
       <c r="C24" s="1"/>
@@ -844,7 +827,7 @@
       <c r="G24" s="1"/>
       <c r="H24" s="1"/>
     </row>
-    <row r="25" spans="1:8">
+    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A25" s="1"/>
       <c r="B25" s="1"/>
       <c r="C25" s="1"/>
@@ -854,7 +837,7 @@
       <c r="G25" s="1"/>
       <c r="H25" s="1"/>
     </row>
-    <row r="26" spans="1:8">
+    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A26" s="1"/>
       <c r="B26" s="1"/>
       <c r="C26" s="1"/>
@@ -864,7 +847,7 @@
       <c r="G26" s="1"/>
       <c r="H26" s="1"/>
     </row>
-    <row r="27" spans="1:8">
+    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A27" s="1"/>
       <c r="B27" s="1"/>
       <c r="C27" s="1"/>
@@ -874,7 +857,7 @@
       <c r="G27" s="1"/>
       <c r="H27" s="1"/>
     </row>
-    <row r="28" spans="1:8">
+    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A28" s="1"/>
       <c r="B28" s="1"/>
       <c r="C28" s="1"/>
@@ -884,7 +867,7 @@
       <c r="G28" s="1"/>
       <c r="H28" s="1"/>
     </row>
-    <row r="29" spans="1:8">
+    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A29" s="1"/>
       <c r="B29" s="1"/>
       <c r="C29" s="1"/>
@@ -894,7 +877,7 @@
       <c r="G29" s="1"/>
       <c r="H29" s="1"/>
     </row>
-    <row r="30" spans="1:8">
+    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A30" s="1"/>
       <c r="B30" s="1"/>
       <c r="C30" s="1"/>
@@ -904,7 +887,7 @@
       <c r="G30" s="1"/>
       <c r="H30" s="1"/>
     </row>
-    <row r="31" spans="1:8">
+    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A31" s="1"/>
       <c r="B31" s="1"/>
       <c r="C31" s="1"/>
@@ -914,7 +897,7 @@
       <c r="G31" s="1"/>
       <c r="H31" s="1"/>
     </row>
-    <row r="32" spans="1:8">
+    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A32" s="1"/>
       <c r="B32" s="1"/>
       <c r="C32" s="1"/>
@@ -924,7 +907,7 @@
       <c r="G32" s="1"/>
       <c r="H32" s="1"/>
     </row>
-    <row r="33" spans="1:8">
+    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A33" s="1"/>
       <c r="B33" s="1"/>
       <c r="C33" s="1"/>
@@ -934,7 +917,7 @@
       <c r="G33" s="1"/>
       <c r="H33" s="1"/>
     </row>
-    <row r="34" spans="1:8">
+    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A34" s="1"/>
       <c r="B34" s="1"/>
       <c r="C34" s="1"/>
@@ -944,7 +927,7 @@
       <c r="G34" s="1"/>
       <c r="H34" s="1"/>
     </row>
-    <row r="35" spans="1:8">
+    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A35" s="1"/>
       <c r="B35" s="1"/>
       <c r="C35" s="1"/>
@@ -954,7 +937,7 @@
       <c r="G35" s="1"/>
       <c r="H35" s="1"/>
     </row>
-    <row r="36" spans="1:8">
+    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A36" s="1"/>
       <c r="B36" s="1"/>
       <c r="C36" s="1"/>
@@ -964,7 +947,7 @@
       <c r="G36" s="1"/>
       <c r="H36" s="1"/>
     </row>
-    <row r="37" spans="1:8">
+    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A37" s="1"/>
       <c r="B37" s="1"/>
       <c r="C37" s="1"/>
@@ -974,7 +957,7 @@
       <c r="G37" s="1"/>
       <c r="H37" s="1"/>
     </row>
-    <row r="38" spans="1:8">
+    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A38" s="1"/>
       <c r="B38" s="1"/>
       <c r="C38" s="1"/>
@@ -984,7 +967,7 @@
       <c r="G38" s="1"/>
       <c r="H38" s="1"/>
     </row>
-    <row r="39" spans="1:8">
+    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A39" s="1"/>
       <c r="B39" s="1"/>
       <c r="C39" s="1"/>
@@ -994,7 +977,7 @@
       <c r="G39" s="1"/>
       <c r="H39" s="1"/>
     </row>
-    <row r="40" spans="1:8">
+    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A40" s="1"/>
       <c r="B40" s="1"/>
       <c r="C40" s="1"/>

</xml_diff>